<commit_message>
Fix JsonDataManager can load and save array
</commit_message>
<xml_diff>
--- a/Data/Stage/Stage.xlsx
+++ b/Data/Stage/Stage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HavePoop\Desktop\Study\BuildingBreaker\Data\Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D186FD-EE06-4EFD-92EF-4E15F17BE785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD3EFEB-325C-4700-9E82-0B959AF850EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6290" yWindow="4420" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>All</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,6 +42,13 @@
   <si>
     <t>StageID</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxStart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsOpen</t>
   </si>
 </sst>
 </file>
@@ -405,150 +412,300 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731530C-0039-42AC-944F-DD348182ED49}">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" style="1" customWidth="1"/>
-    <col min="3" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.58203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.58203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.08203125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="1"/>
+    <col min="1" max="2" width="25.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="1" customWidth="1"/>
+    <col min="4" max="9" width="15" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.58203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.25" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.58203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.08203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>22</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix EventManager has index
</commit_message>
<xml_diff>
--- a/Data/Stage/Stage.xlsx
+++ b/Data/Stage/Stage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HavePoop\Desktop\Study\BuildingBreaker\Data\Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD3EFEB-325C-4700-9E82-0B959AF850EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C65A85-7DDD-4317-960C-D64D24965258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6290" yWindow="4420" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,11 +44,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MaxStart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>IsOpen</t>
   </si>
   <si>
-    <t>IsOpen</t>
+    <t>MaxStar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -449,10 +449,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>